<commit_message>
Testes finais bem sucedidos.
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\projeto-tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C792C12A-0992-465B-8799-5BE80D6A75A1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C21AB50D-F1CA-4CE2-89D3-F49817372D6A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15405" windowHeight="11340" activeTab="2" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -18,6 +13,7 @@
     <sheet name="PesquisaBarra" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:L5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -505,7 +501,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Codigo refatorado de acordo com as boas praticas em tdd e pagefactory.
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\git\projeto-tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\projeto-tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E55FC83-1679-4972-8BAF-A00BFE0AB7ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D769DB-810D-4664-BD62-B1FFB0053BE8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -574,7 +574,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refatorando comandos de wait.
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3AF9AEA0-94C1-46C4-903B-F41BC3C497B7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\projeto-tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11774A19-BCB5-4B49-8578-1C9281F1F55F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15525" windowHeight="11820" firstSheet="2" activeTab="2" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,6 @@
     <sheet name="Pagamento" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A7:C8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>txt_UserName</t>
   </si>
@@ -186,6 +190,9 @@
   </si>
   <si>
     <t>HP Chromebook 14 G1(ES)</t>
+  </si>
+  <si>
+    <t>iiiiioooooppu</t>
   </si>
 </sst>
 </file>
@@ -575,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B732072B-4DFA-4889-A7A4-3C1058C30EFF}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -639,7 +646,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
@@ -793,7 +800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BBC43E-FC47-4208-85C2-FA45BE08B035}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Organização das tabelas de massa.
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\projeto-tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\git\projeto-tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11774A19-BCB5-4B49-8578-1C9281F1F55F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71209D5-71D9-4FB6-9E27-7920CA518E40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -28,43 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
-  <si>
-    <t>txt_UserName</t>
-  </si>
-  <si>
-    <t>txt_Email</t>
-  </si>
-  <si>
-    <t>txt_Password</t>
-  </si>
-  <si>
-    <t>txt_ConfirmPassword</t>
-  </si>
-  <si>
-    <t>txt_FirstName</t>
-  </si>
-  <si>
-    <t>txt_LastName</t>
-  </si>
-  <si>
-    <t>txt_Telefone</t>
-  </si>
-  <si>
-    <t>combo_Pais</t>
-  </si>
-  <si>
-    <t>txt_Cidade</t>
-  </si>
-  <si>
-    <t>txt_Endereco</t>
-  </si>
-  <si>
-    <t>txt_Estado</t>
-  </si>
-  <si>
-    <t>txt_Cep</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>lucascarvalho</t>
   </si>
@@ -102,97 +66,154 @@
     <t>102030400Lcc</t>
   </si>
   <si>
-    <t>txt_UserNameCat</t>
-  </si>
-  <si>
-    <t>txt_PasswordCat</t>
-  </si>
-  <si>
-    <t>txt_QuantidadeCat</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
     <t>HP</t>
   </si>
   <si>
-    <t>txt_PesquisaBarraErro</t>
-  </si>
-  <si>
-    <t>txt_PesquisaBarra</t>
-  </si>
-  <si>
     <t>fones</t>
   </si>
   <si>
-    <t>txt_UserNamePay</t>
-  </si>
-  <si>
-    <t>txt_PasswordPay</t>
-  </si>
-  <si>
-    <t>condicao_Assert</t>
-  </si>
-  <si>
-    <t>msg_Assert</t>
-  </si>
-  <si>
-    <t>HP ROAR MINI WIRELESS SPEAKER</t>
-  </si>
-  <si>
     <t>Pesquisa efetuada com sucesso!</t>
   </si>
   <si>
-    <t>condicao_AssertMassa</t>
-  </si>
-  <si>
-    <t>msg_AssertMassa</t>
-  </si>
-  <si>
-    <t>ORDER PAYMENT</t>
-  </si>
-  <si>
     <t>Compra efetuada com sucesso!</t>
   </si>
   <si>
-    <t>msg_AssertCadastro</t>
-  </si>
-  <si>
     <t>Cadastro efetuado com sucesso!</t>
   </si>
   <si>
-    <t>condicao_AssertMassaErro</t>
-  </si>
-  <si>
-    <t>msg_AssertMassaErro</t>
-  </si>
-  <si>
     <t>QTY: 10</t>
   </si>
   <si>
     <t>Quantidade errada.</t>
   </si>
   <si>
-    <t>condicao_AssertCadastroErro</t>
-  </si>
-  <si>
-    <t>msg_AssertCadastroErro</t>
-  </si>
-  <si>
     <t>Passwords do not match</t>
   </si>
   <si>
     <t>A senha nao e a mesma!</t>
   </si>
   <si>
-    <t>clica_Produto</t>
-  </si>
-  <si>
     <t>HP Chromebook 14 G1(ES)</t>
   </si>
   <si>
-    <t>iiiiioooooppu</t>
+    <t>Thank you for buying with Advantage</t>
+  </si>
+  <si>
+    <t>HP ZBOOK 17 G2 MOBILE WORKSTATION</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Pagina de Cadastro</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Telefone</t>
+  </si>
+  <si>
+    <t>Pais</t>
+  </si>
+  <si>
+    <t>Cidade</t>
+  </si>
+  <si>
+    <t>Endereco</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Cep</t>
+  </si>
+  <si>
+    <t>Asserts</t>
+  </si>
+  <si>
+    <t>CondicaoAssertCadastroErro</t>
+  </si>
+  <si>
+    <t>MensagemAssertCadastroErro</t>
+  </si>
+  <si>
+    <t>MensagemAssertCadastroSucesso</t>
+  </si>
+  <si>
+    <t>ConfirmInvalidPassword</t>
+  </si>
+  <si>
+    <t>lucascarvalh7</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Seleciona Produto</t>
+  </si>
+  <si>
+    <t>Produto</t>
+  </si>
+  <si>
+    <t>Altera qunatidade de produtos</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
+    <t>MensagemAssertMassaSucesso</t>
+  </si>
+  <si>
+    <t>CondicaoAssertMassaSucesso</t>
+  </si>
+  <si>
+    <t>CondicaoAssertMassaErro</t>
+  </si>
+  <si>
+    <t>MensagemAssertMassaErro</t>
+  </si>
+  <si>
+    <t>UserNamePay</t>
+  </si>
+  <si>
+    <t>PasswordPay</t>
+  </si>
+  <si>
+    <t>Logar no Pay</t>
+  </si>
+  <si>
+    <t>Pesquisa Inexistente</t>
+  </si>
+  <si>
+    <t>Pesquisa Estimada Existente</t>
+  </si>
+  <si>
+    <t>PesquisaBarra</t>
+  </si>
+  <si>
+    <t>PesquisaBarraErro</t>
+  </si>
+  <si>
+    <t>CondicaoAssertBarra</t>
+  </si>
+  <si>
+    <t>MensagemAssertBarra</t>
   </si>
 </sst>
 </file>
@@ -257,14 +278,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -580,21 +619,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B732072B-4DFA-4889-A7A4-3C1058C30EFF}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
@@ -603,112 +641,193 @@
     <col min="13" max="13" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
-      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{39EDB8B1-25FF-40AC-8F4C-2FC02CCB478C}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{39EDB8B1-25FF-40AC-8F4C-2FC02CCB478C}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -717,80 +836,131 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B33322F-19DE-45EB-B55A-70A3D3B1968A}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="34.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>53</v>
-      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -798,61 +968,95 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BBC43E-FC47-4208-85C2-FA45BE08B035}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="5" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D883A96-26C0-4A40-9A6E-BCEE8A84DD95}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,22 +1066,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="A1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
+      <c r="A2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Comentários adicionados nas linhas de código para melhor compreensão.
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\git\projeto-tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA13768F-0B99-421A-8A15-A993C3EEBC61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FB7CB5D5-2C69-474E-9BE8-984562FBDE04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15435" windowHeight="11820" activeTab="2" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -19,6 +14,7 @@
     <sheet name="Pagamento" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A4:D14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -281,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -308,6 +304,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -627,7 +626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B732072B-4DFA-4889-A7A4-3C1058C30EFF}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -976,7 +975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BBC43E-FC47-4208-85C2-FA45BE08B035}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1019,7 +1018,7 @@
       <c r="A3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C3" s="1"/>

</xml_diff>

<commit_message>
Correções para o workspace da rsi.
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FB7CB5D5-2C69-474E-9BE8-984562FBDE04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\jee\projeto-tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB3483A-1DE6-4F45-891D-E271EF6E0A0C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15435" windowHeight="11820" activeTab="2" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
+    <workbookView xWindow="3585" yWindow="1635" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,6 @@
     <sheet name="Pagamento" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A4:D14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
   <si>
     <t>lucascarvalho</t>
   </si>
@@ -98,9 +102,6 @@
     <t>Thank you for buying with Advantage</t>
   </si>
   <si>
-    <t>HP ZBOOK 17 G2 MOBILE WORKSTATION</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -212,14 +213,20 @@
     <t>EscolheProduto</t>
   </si>
   <si>
-    <t>HP ZBook 17 G2 Mobile Workstation</t>
+    <t>lucascarvalh9</t>
+  </si>
+  <si>
+    <t>HP Z3600 Wireless Mouse</t>
+  </si>
+  <si>
+    <t>HP Z3600 WIRELESS MOUSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +244,13 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -297,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -306,7 +320,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -627,7 +641,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,27 +662,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="1"/>
       <c r="E1" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>20</v>
@@ -676,15 +690,15 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>21</v>
@@ -692,7 +706,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -700,7 +714,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>17</v>
@@ -708,7 +722,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -720,7 +734,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
@@ -732,7 +746,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -744,7 +758,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -756,7 +770,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
@@ -768,7 +782,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>6</v>
@@ -780,7 +794,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
@@ -792,7 +806,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>8</v>
@@ -804,7 +818,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -816,7 +830,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>10</v>
@@ -858,25 +872,25 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="1"/>
       <c r="D1" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>16</v>
@@ -884,14 +898,14 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>23</v>
@@ -902,7 +916,7 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>19</v>
@@ -910,12 +924,12 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="1"/>
       <c r="D5" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>18</v>
@@ -923,7 +937,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>22</v>
@@ -941,7 +955,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="1"/>
@@ -950,7 +964,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>12</v>
@@ -975,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BBC43E-FC47-4208-85C2-FA45BE08B035}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,40 +1004,40 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="1"/>
       <c r="D1" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>62</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>15</v>
@@ -1036,7 +1050,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="1"/>
@@ -1045,7 +1059,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>14</v>
@@ -1078,13 +1092,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1092,7 +1106,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Refatoração de boas praticas.
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\jee\projeto-tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\git\projeto-tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB3483A-1DE6-4F45-891D-E271EF6E0A0C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8F5456-2F5F-4691-9B7D-345DE8986199}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="1635" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -213,13 +213,13 @@
     <t>EscolheProduto</t>
   </si>
   <si>
-    <t>lucascarvalh9</t>
-  </si>
-  <si>
     <t>HP Z3600 Wireless Mouse</t>
   </si>
   <si>
     <t>HP Z3600 WIRELESS MOUSE</t>
+  </si>
+  <si>
+    <t>lucascarval37</t>
   </si>
 </sst>
 </file>
@@ -314,13 +314,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -640,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B732072B-4DFA-4889-A7A4-3C1058C30EFF}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,23 +661,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="9"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -692,7 +692,7 @@
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1"/>
@@ -871,15 +871,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="9"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="9"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -923,10 +923,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="1"/>
       <c r="D5" s="4" t="s">
         <v>49</v>
@@ -954,10 +954,10 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -989,7 +989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BBC43E-FC47-4208-85C2-FA45BE08B035}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1003,15 +1003,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="9"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="9"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1025,7 +1025,7 @@
         <v>58</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1033,7 +1033,7 @@
         <v>60</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="4" t="s">
@@ -1049,10 +1049,10 @@
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1091,10 +1091,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Testes rodando com sucesso.
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/testData/MassaDeDados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\git\projeto-tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas.correia\git\projeto-tdd\src\main\java\br\com\rsinet\hub_tdd\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E65EFAC-5681-4841-A15A-F9F346B4ED3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BC5C07-C1BB-4DA3-8F38-C0C00D987BD1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{0BA68D2D-8DA9-4321-A4B9-3BA70DFA1B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -219,7 +219,7 @@
     <t>HP Z3600 WIRELESS MOUSE</t>
   </si>
   <si>
-    <t>lucascarval38</t>
+    <t>lucascarval43</t>
   </si>
 </sst>
 </file>

</xml_diff>